<commit_message>
Modifying my keyword framework to be a hybrid driven framework
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/hs/keyword/scenarios/hubspot_scenarios.xlsx
+++ b/src/main/java/com/qa/hs/keyword/scenarios/hubspot_scenarios.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
   <si>
     <t>action</t>
   </si>
@@ -104,12 +104,6 @@
   </si>
   <si>
     <t>firefox</t>
-  </si>
-  <si>
-    <t>samir95</t>
-  </si>
-  <si>
-    <t>P@$$w0rd</t>
   </si>
   <si>
     <t>http://parabank.parasoft.com/parabank/index.htm</t>
@@ -135,7 +129,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -182,6 +176,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -218,7 +218,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -230,6 +230,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -502,7 +503,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -512,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -573,15 +574,15 @@
         <v>12</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
@@ -589,8 +590,8 @@
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>28</v>
+      <c r="E4" s="9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -598,7 +599,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -606,8 +607,8 @@
       <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>29</v>
+      <c r="E5" s="9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -618,7 +619,7 @@
         <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
@@ -635,7 +636,7 @@
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
         <v>24</v>
@@ -652,13 +653,13 @@
         <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
         <v>26</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -682,9 +683,10 @@
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" display="naveenanimation20@gmail.com"/>
     <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E5" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId3" display="P@$$w0rd"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>